<commit_message>
add auto column width
</commit_message>
<xml_diff>
--- a/rakuten.xlsx
+++ b/rakuten.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
   <si>
     <t>轉入頂新</t>
   </si>
@@ -38,6 +38,51 @@
   </si>
   <si>
     <t>收貨人</t>
+  </si>
+  <si>
+    <t>卡拉蝦原味</t>
+  </si>
+  <si>
+    <t>卡拉蝦辣味</t>
+  </si>
+  <si>
+    <t>卡拉魷原味</t>
+  </si>
+  <si>
+    <t>卡拉魷辣味</t>
+  </si>
+  <si>
+    <t>卡拉魷芥末</t>
+  </si>
+  <si>
+    <t>卡拉蟹原味</t>
+  </si>
+  <si>
+    <t>卡拉蟹辣味</t>
+  </si>
+  <si>
+    <t>卡拉龍珠原味</t>
+  </si>
+  <si>
+    <t>卡拉龍珠辣味</t>
+  </si>
+  <si>
+    <t>卡拉龍珠芥末</t>
+  </si>
+  <si>
+    <t>卡拉小卷原味</t>
+  </si>
+  <si>
+    <t>卡拉小卷芥末</t>
+  </si>
+  <si>
+    <t>虱目魚薄燒脆片海苔</t>
+  </si>
+  <si>
+    <t>虱目魚薄燒脆片黑胡椒</t>
+  </si>
+  <si>
+    <t>虱目魚薄燒脆片蒜香</t>
   </si>
   <si>
     <t>贈送</t>
@@ -469,14 +514,54 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:AJ9"/>
+  <dimension ref="A1:AJ9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="9"/>
+    <col customWidth="1" max="2" min="2" width="16"/>
+    <col customWidth="1" max="3" min="3" width="15"/>
+    <col customWidth="1" max="4" min="4" width="9"/>
+    <col customWidth="1" max="5" min="5" width="15"/>
+    <col customWidth="1" max="6" min="6" width="16"/>
+    <col customWidth="1" max="7" min="7" width="9"/>
+    <col customWidth="1" max="8" min="8" width="9"/>
+    <col customWidth="1" max="9" min="9" width="10"/>
+    <col customWidth="1" max="10" min="10" width="10"/>
+    <col customWidth="1" max="11" min="11" width="10"/>
+    <col customWidth="1" max="12" min="12" width="10"/>
+    <col customWidth="1" max="13" min="13" width="10"/>
+    <col customWidth="1" max="14" min="14" width="10"/>
+    <col customWidth="1" max="15" min="15" width="10"/>
+    <col customWidth="1" max="16" min="16" width="11"/>
+    <col customWidth="1" max="17" min="17" width="11"/>
+    <col customWidth="1" max="18" min="18" width="11"/>
+    <col customWidth="1" max="19" min="19" width="11"/>
+    <col customWidth="1" max="20" min="20" width="11"/>
+    <col customWidth="1" max="21" min="21" width="14"/>
+    <col customWidth="1" max="22" min="22" width="15"/>
+    <col customWidth="1" max="23" min="23" width="14"/>
+    <col customWidth="1" max="24" min="24" width="7"/>
+    <col customWidth="1" max="25" min="25" width="7"/>
+    <col customWidth="1" max="26" min="26" width="7"/>
+    <col customWidth="1" max="27" min="27" width="7"/>
+    <col customWidth="1" max="28" min="28" width="9"/>
+    <col customWidth="1" max="29" min="29" width="15"/>
+    <col customWidth="1" max="30" min="30" width="15"/>
+    <col customWidth="1" max="31" min="31" width="38"/>
+    <col customWidth="1" max="32" min="32" width="11"/>
+    <col customWidth="1" max="33" min="33" width="7"/>
+    <col customWidth="1" max="34" min="34" width="11"/>
+    <col customWidth="1" max="35" min="35" width="11"/>
+    <col customWidth="1" max="36" min="36" width="7"/>
+  </cols>
   <sheetData>
+    <row r="1" spans="1:36"/>
+    <row r="2" spans="1:36"/>
     <row r="3" spans="1:36">
       <c r="A3" t="s">
         <v>0</v>
@@ -502,218 +587,263 @@
       <c r="H3" t="s">
         <v>7</v>
       </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W3" t="s">
+        <v>22</v>
+      </c>
       <c r="X3" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="Y3" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="Z3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="AA3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="AB3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="AC3" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="AD3" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="AE3" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="AF3" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="AG3" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="AH3" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="AI3" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="AJ3" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:36">
       <c r="B4" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="AC4" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="AD4" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="AE4" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:36">
       <c r="B5" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="AC5" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="AD5" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="AE5" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:36">
       <c r="B6" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="AC6" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="AD6" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="AE6" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:36">
       <c r="B7" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="H7" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="AC7" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="AD7" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="AE7" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:36">
       <c r="B8" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="G8" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="H8" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="AC8" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="AD8" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="AE8" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:36">
       <c r="B9" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="H9" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="AC9" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="AD9" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="AE9" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>